<commit_message>
date updated to August
</commit_message>
<xml_diff>
--- a/TestCasesOrangeHRM_July2019.xlsx
+++ b/TestCasesOrangeHRM_July2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aodada\Desktop\others\School_of_Software\Manual Testing\classwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aodada\Desktop\gitlesson\teaching\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,18 +35,12 @@
     <t>Project</t>
   </si>
   <si>
-    <t>HRM-July19</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Responsible Person</t>
   </si>
   <si>
-    <t>Alexi</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>Test Scenario: Valid_LoginHRM</t>
+  </si>
+  <si>
+    <t>HRM-August 2019</t>
+  </si>
+  <si>
+    <t>Olawale Obanla</t>
   </si>
 </sst>
 </file>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,12 +610,12 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>43647</v>
@@ -623,304 +623,304 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
         <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
         <v>46</v>
-      </c>
-      <c r="D32" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>